<commit_message>
ev branch under test
</commit_message>
<xml_diff>
--- a/data/input_operation/EV100/OperationScenario_Component_Building.xlsx
+++ b/data/input_operation/EV100/OperationScenario_Component_Building.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_operation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_operation/EV100/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2309F49E-2846-6F42-AB12-F8CFEAA353BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC69E94-3452-3A4E-8F4A-71EF7B9916F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="-18060" windowWidth="25880" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Bui" sheetId="1" r:id="rId1"/>
@@ -920,7 +920,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1033,7 +1033,7 @@
         <v>21000</v>
       </c>
       <c r="Q2">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1086,7 +1086,7 @@
         <v>21000</v>
       </c>
       <c r="Q3">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1139,7 +1139,7 @@
         <v>21000</v>
       </c>
       <c r="Q4">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>